<commit_message>
2nd figure added in optimization.tex
</commit_message>
<xml_diff>
--- a/other/PSU_specs.xlsx
+++ b/other/PSU_specs.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="9630"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="9630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="current specs" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Speed (ns/bit)</t>
   </si>
@@ -36,6 +37,15 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>In-plane MTJ</t>
+  </si>
+  <si>
+    <t>Perpendicular MTJ</t>
+  </si>
+  <si>
+    <t>Write Pulse Width (ns)</t>
   </si>
 </sst>
 </file>
@@ -73,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -82,6 +92,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -124,7 +137,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -870,11 +882,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="104030208"/>
-        <c:axId val="104032512"/>
+        <c:axId val="58267904"/>
+        <c:axId val="58275328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104030208"/>
+        <c:axId val="58267904"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -898,17 +910,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="104032512"/>
+        <c:crossAx val="58275328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104032512"/>
+        <c:axId val="58275328"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -936,7 +947,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -947,20 +957,19 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="104030208"/>
+        <c:crossAx val="58267904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1130,11 +1139,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="102673024"/>
-        <c:axId val="104870656"/>
+        <c:axId val="58301824"/>
+        <c:axId val="58394496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102673024"/>
+        <c:axId val="58301824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1161,17 +1170,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104870656"/>
+        <c:crossAx val="58394496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104870656"/>
+        <c:axId val="58394496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,8 +1210,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.2038567493112955E-2"/>
-              <c:y val="5.0029009531703278E-2"/>
+              <c:x val="2.2038567493113004E-2"/>
+              <c:y val="5.0029009531703292E-2"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -1216,7 +1224,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="102673024"/>
+        <c:crossAx val="58301824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1225,7 +1233,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1467,12 +1475,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="58561280"/>
-        <c:axId val="58555392"/>
+        <c:axId val="67350528"/>
+        <c:axId val="67353600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58561280"/>
+        <c:axId val="67350528"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1504,19 +1511,19 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.31233738807117251"/>
-              <c:y val="0.83102850061957867"/>
+              <c:y val="0.83102850061958033"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="58555392"/>
+        <c:crossAx val="67353600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58555392"/>
+        <c:axId val="67353600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1548,7 +1555,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.8165304268846504E-2"/>
+              <c:x val="1.8165304268846529E-2"/>
               <c:y val="3.6978559498244551E-2"/>
             </c:manualLayout>
           </c:layout>
@@ -1561,7 +1568,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58561280"/>
+        <c:crossAx val="67350528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1570,7 +1577,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1880,12 +1887,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="65762048"/>
-        <c:axId val="65760256"/>
+        <c:axId val="72368512"/>
+        <c:axId val="72370432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65762048"/>
+        <c:axId val="72368512"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1912,17 +1918,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="65760256"/>
+        <c:crossAx val="72370432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65760256"/>
+        <c:axId val="72370432"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1945,7 +1950,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1956,7 +1960,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="65762048"/>
+        <c:crossAx val="72368512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1965,7 +1969,1602 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="33"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16452645054245632"/>
+          <c:y val="5.6717852797135988E-2"/>
+          <c:w val="0.75166798973016657"/>
+          <c:h val="0.71500165927534964"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In-plane MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$4:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>114.20335508047508</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115.85847616859793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.92737752875145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120.58739356323456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.13408160921206</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>129.09944487358055</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136.54748977013327</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148.96089793105446</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173.78771425289688</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>248.26816321842412</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>285.50838770118776</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>347.57542850579375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>397.22906114947858</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Perpendicular MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$D$4:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>36.114271848726339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.637667092910789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.291911148141338</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.133082076294897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.254643313832986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.824829046386306</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.180107645216282</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.105571976599578</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.956500639366176</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.509286627665972</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.285679621815859</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>109.91300127873235</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>125.61485860426555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="72749440"/>
+        <c:axId val="72752512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="72749440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Write Pulse Width (ns)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72752512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="72752512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="400"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Switching </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0"/>
+                  <a:t>Current (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1400" b="0">
+                    <a:latin typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0">
+                    <a:latin typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72749440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34836111111111112"/>
+          <c:y val="0.10482034573264552"/>
+          <c:w val="0.56572221387858002"/>
+          <c:h val="0.21625365794792908"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="33"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20447884185417009"/>
+          <c:y val="5.6717852797135988E-2"/>
+          <c:w val="0.75347944754768981"/>
+          <c:h val="0.71500165927534964"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In-plane MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$F$4:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$4:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.39127218934911223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36242603550295854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33376479289940814</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30536770921386291</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27736686390532539</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22374260355029582</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19970414201183426</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18121301775147922</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18491124260355024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1956360946745562</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21745562130177506</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.23668639053254434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Perpendicular MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$F$4:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$4:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.9127218934911237E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.624260355029587E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3376479289940843E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0536770921386312E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7736686390532551E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2374260355029589E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9970414201183433E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8121301775147931E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8491124260355034E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9563609467455622E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1745562130177518E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3668639053254441E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="72778880"/>
+        <c:axId val="72815360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="72778880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Write Pulse Width (ns)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="72815360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="72815360"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="1.0000000000000005E-2"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Energy per</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> cell </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0"/>
+                  <a:t>(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0">
+                    <a:latin typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>pJ)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72778880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16502777777777777"/>
+          <c:y val="6.3153616214639899E-2"/>
+          <c:w val="0.56572221387858046"/>
+          <c:h val="0.21625365794792914"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="33"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18960498276273482"/>
+          <c:y val="5.6717852797135988E-2"/>
+          <c:w val="0.72658948979339966"/>
+          <c:h val="0.71500165927534964"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In-plane MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$4:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>114.20335508047508</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115.85847616859793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.92737752875145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120.58739356323456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.13408160921206</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>129.09944487358055</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136.54748977013327</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148.96089793105446</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173.78771425289688</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>248.26816321842412</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>285.50838770118776</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>347.57542850579375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>397.22906114947858</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Perpendicular MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$D$4:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>36.114271848726339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.637667092910789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.291911148141338</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.133082076294897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.254643313832986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.824829046386306</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.180107645216282</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.105571976599578</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.956500639366176</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.509286627665972</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.285679621815859</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>109.91300127873235</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>125.61485860426555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="76658176"/>
+        <c:axId val="77970048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="76658176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Write Pulse Width (ns)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77970048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="77970048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="400"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Switching Current (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1400" b="1">
+                    <a:latin typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1">
+                    <a:latin typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76658176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32746262516558522"/>
+          <c:y val="4.9896206156048818E-2"/>
+          <c:w val="0.56572221387858046"/>
+          <c:h val="0.19100095442615128"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="33"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21237245344331959"/>
+          <c:y val="5.6717852797135988E-2"/>
+          <c:w val="0.74078106903303764"/>
+          <c:h val="0.71500165927534964"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In-plane MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$F$4:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$4:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.39127218934911223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36242603550295854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33376479289940814</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30536770921386291</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27736686390532539</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22374260355029582</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19970414201183426</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18121301775147922</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18491124260355024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1956360946745562</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21745562130177506</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.23668639053254434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Perpendicular MTJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$F$4:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$4:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.9127218934911237E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.624260355029587E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3376479289940843E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0536770921386312E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7736686390532551E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2374260355029589E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9970414201183433E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8121301775147931E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8491124260355034E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9563609467455622E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1745562130177518E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3668639053254441E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="78314496"/>
+        <c:axId val="95696384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="78314496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Write Pulse Width (ns)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="95696384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="95696384"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="1.0000000000000005E-2"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Cell</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                  <a:t> Switching Energy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1">
+                    <a:latin typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>pJ)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0"/>
+              <c:y val="4.1450582036024107E-2"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78314496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20264519819637952"/>
+          <c:y val="3.7041761815188201E-2"/>
+          <c:w val="0.56572221387858102"/>
+          <c:h val="0.21625365794792922"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2065,16 +3664,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2091,6 +3690,256 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="2466974"/>
+          <a:ext cx="685800" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1"/>
+            <a:t>(a)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4533900" y="2466974"/>
+          <a:ext cx="685800" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1"/>
+            <a:t>(b)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2383,8 +4232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" activeCellId="2" sqref="A5:A17 G5:G17 K5:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2399,13 +4248,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
@@ -3271,12 +5120,317 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="5">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>114.20335508047508</v>
+      </c>
+      <c r="D4" s="3">
+        <v>36.114271848726339</v>
+      </c>
+      <c r="F4" s="5">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0.39127218934911223</v>
+      </c>
+      <c r="H4">
+        <v>3.9127218934911237E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="5">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>115.85847616859793</v>
+      </c>
+      <c r="D5" s="3">
+        <v>36.637667092910789</v>
+      </c>
+      <c r="F5" s="5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>0.36242603550295854</v>
+      </c>
+      <c r="H5">
+        <v>3.624260355029587E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>117.92737752875145</v>
+      </c>
+      <c r="D6" s="3">
+        <v>37.291911148141338</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>0.33376479289940814</v>
+      </c>
+      <c r="H6">
+        <v>3.3376479289940843E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="5">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>120.58739356323456</v>
+      </c>
+      <c r="D7" s="3">
+        <v>38.133082076294897</v>
+      </c>
+      <c r="F7" s="5">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>0.30536770921386291</v>
+      </c>
+      <c r="H7">
+        <v>3.0536770921386312E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>124.13408160921206</v>
+      </c>
+      <c r="D8" s="3">
+        <v>39.254643313832986</v>
+      </c>
+      <c r="F8" s="5">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>0.27736686390532539</v>
+      </c>
+      <c r="H8">
+        <v>2.7736686390532551E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>129.09944487358055</v>
+      </c>
+      <c r="D9" s="3">
+        <v>40.824829046386306</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="H9">
+        <v>2.5000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="5">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>136.54748977013327</v>
+      </c>
+      <c r="D10" s="3">
+        <v>43.180107645216282</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>0.22374260355029582</v>
+      </c>
+      <c r="H10">
+        <v>2.2374260355029589E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="5">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>148.96089793105446</v>
+      </c>
+      <c r="D11" s="3">
+        <v>47.105571976599578</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>0.19970414201183426</v>
+      </c>
+      <c r="H11">
+        <v>1.9970414201183433E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>173.78771425289688</v>
+      </c>
+      <c r="D12" s="3">
+        <v>54.956500639366176</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.18121301775147922</v>
+      </c>
+      <c r="H12">
+        <v>1.8121301775147931E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>248.26816321842412</v>
+      </c>
+      <c r="D13" s="3">
+        <v>78.509286627665972</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.18491124260355024</v>
+      </c>
+      <c r="H13">
+        <v>1.8491124260355034E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>285.50838770118776</v>
+      </c>
+      <c r="D14" s="3">
+        <v>90.285679621815859</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="G14">
+        <v>0.1956360946745562</v>
+      </c>
+      <c r="H14">
+        <v>1.9563609467455622E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C15" s="3">
+        <v>347.57542850579375</v>
+      </c>
+      <c r="D15" s="3">
+        <v>109.91300127873235</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="G15">
+        <v>0.21745562130177506</v>
+      </c>
+      <c r="H15">
+        <v>2.1745562130177518E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>397.22906114947858</v>
+      </c>
+      <c r="D16" s="3">
+        <v>125.61485860426555</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>0.23668639053254434</v>
+      </c>
+      <c r="H16">
+        <v>2.3668639053254441E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>